<commit_message>
veel shit waaronder tier 2 flame tower upgrades
</commit_message>
<xml_diff>
--- a/data/towdef/upgrade paths.xlsx
+++ b/data/towdef/upgrade paths.xlsx
@@ -7,20 +7,18 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Machine gun" sheetId="1" r:id="rId1"/>
-    <sheet name="Flame thrower" sheetId="5" r:id="rId2"/>
-    <sheet name="Rocket launcher" sheetId="4" r:id="rId3"/>
+    <sheet name="Machine gun tower" sheetId="1" r:id="rId1"/>
+    <sheet name="Flame tower" sheetId="5" r:id="rId2"/>
+    <sheet name="Rocket tower" sheetId="4" r:id="rId3"/>
     <sheet name="Freezing tower" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
-  <si>
-    <t>Machine gun</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>U0.0.0.0</t>
   </si>
@@ -49,9 +47,6 @@
     <t>U0.0.0.4</t>
   </si>
   <si>
-    <t>Flame thrower</t>
-  </si>
-  <si>
     <t>U0.0.1.0</t>
   </si>
   <si>
@@ -67,7 +62,37 @@
     <t>Freezing tower</t>
   </si>
   <si>
-    <t>Rocket launcher</t>
+    <t>U0.0.1.4</t>
+  </si>
+  <si>
+    <t>U0.0.1.5</t>
+  </si>
+  <si>
+    <t>U0.0.1.6</t>
+  </si>
+  <si>
+    <t>U0.0.1.7</t>
+  </si>
+  <si>
+    <t>U0.0.1.9</t>
+  </si>
+  <si>
+    <t>U0.0.1.10</t>
+  </si>
+  <si>
+    <t>U0.0.1.8</t>
+  </si>
+  <si>
+    <t>U0.0.1.11</t>
+  </si>
+  <si>
+    <t>Flame tower</t>
+  </si>
+  <si>
+    <t>Machine gun tower</t>
+  </si>
+  <si>
+    <t>Rocket tower</t>
   </si>
 </sst>
 </file>
@@ -535,6 +560,241 @@
           <a:avLst>
             <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Rechte verbindingslijn met pijl 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="295275"/>
+          <a:ext cx="657225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Rechte verbindingslijn met pijl 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="476250"/>
+          <a:ext cx="657225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Rechte verbindingslijn met pijl 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="857250"/>
+          <a:ext cx="657225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Rechte verbindingslijn met pijl 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="1057275"/>
+          <a:ext cx="657225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Rechte verbindingslijn met pijl 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3857625" y="1447800"/>
+          <a:ext cx="657225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -1338,7 +1598,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,40 +1608,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1392,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,34 +1665,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1456,18 +1744,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1491,18 +1779,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>